<commit_message>
fixes for players with real clubs
</commit_message>
<xml_diff>
--- a/database/_legacy-data/clubs.xlsx
+++ b/database/_legacy-data/clubs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="3360" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3720" yWindow="0" windowWidth="3360" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mannschaft" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="325">
   <si>
     <t>Dritte III</t>
   </si>
@@ -907,6 +907,93 @@
   </si>
   <si>
     <t>NK Croatia 70</t>
+  </si>
+  <si>
+    <t>SSV Erkrath 1919 e.V.</t>
+  </si>
+  <si>
+    <t>SV Eintracht Solingen</t>
+  </si>
+  <si>
+    <t>SV Eintracht</t>
+  </si>
+  <si>
+    <t>Reusrath</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Tesla</t>
+  </si>
+  <si>
+    <t>SC Germania Reusrath 1913 e.V.</t>
+  </si>
+  <si>
+    <t>SV Eintracht Haarbrück-Jakobsberg</t>
+  </si>
+  <si>
+    <t>Haarbrück</t>
+  </si>
+  <si>
+    <t>DJK Sportfreunde Gerresheim 1923 e.V.</t>
+  </si>
+  <si>
+    <t>Sportfr. Gerresheim</t>
+  </si>
+  <si>
+    <t>Spvgg 1904 e.V. Mössingen</t>
+  </si>
+  <si>
+    <t>Mössingen</t>
+  </si>
+  <si>
+    <t>SV 1930 Issum e.V.</t>
+  </si>
+  <si>
+    <t>Issum</t>
+  </si>
+  <si>
+    <t>FSV Gevelsberg e.V.</t>
+  </si>
+  <si>
+    <t>Gevelsberg</t>
+  </si>
+  <si>
+    <t>Verein für Sport und Freizeit von 1975 Düsseldorf-Süd e.V.</t>
+  </si>
+  <si>
+    <t>SFD75</t>
+  </si>
+  <si>
+    <t>Sportring Eller 1892 e.V.</t>
+  </si>
+  <si>
+    <t>Sportring</t>
+  </si>
+  <si>
+    <t>TuS Homberg 1912 e.V.</t>
+  </si>
+  <si>
+    <t>Homberg</t>
+  </si>
+  <si>
+    <t>DJK Sparta Bilk e.V.</t>
+  </si>
+  <si>
+    <t>Sparta Bilk</t>
+  </si>
+  <si>
+    <t>Angermund</t>
+  </si>
+  <si>
+    <t>TV Angermund 1909 e.V.</t>
+  </si>
+  <si>
+    <t>DJK TuSA 06 Düsseldorf e.V.</t>
+  </si>
+  <si>
+    <t>Tusa</t>
   </si>
 </sst>
 </file>
@@ -1751,19 +1838,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T79"/>
+  <dimension ref="A1:T92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B80" sqref="B80"/>
+      <selection pane="bottomRight" activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
@@ -3992,7 +4079,13 @@
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>77</v>
+      </c>
       <c r="B77" t="s">
+        <v>296</v>
+      </c>
+      <c r="C77" t="s">
         <v>293</v>
       </c>
       <c r="S77">
@@ -4003,13 +4096,252 @@
       </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>78</v>
+      </c>
       <c r="B78" t="s">
         <v>294</v>
       </c>
+      <c r="C78" t="s">
+        <v>301</v>
+      </c>
+      <c r="S78">
+        <v>1</v>
+      </c>
+      <c r="T78">
+        <v>1</v>
+      </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>79</v>
+      </c>
       <c r="B79" t="s">
         <v>295</v>
+      </c>
+      <c r="C79" t="s">
+        <v>300</v>
+      </c>
+      <c r="S79">
+        <v>1</v>
+      </c>
+      <c r="T79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>297</v>
+      </c>
+      <c r="C80" t="s">
+        <v>298</v>
+      </c>
+      <c r="S80">
+        <v>1</v>
+      </c>
+      <c r="T80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>302</v>
+      </c>
+      <c r="C81" t="s">
+        <v>299</v>
+      </c>
+      <c r="S81">
+        <v>1</v>
+      </c>
+      <c r="T81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>303</v>
+      </c>
+      <c r="C82" t="s">
+        <v>304</v>
+      </c>
+      <c r="S82">
+        <v>1</v>
+      </c>
+      <c r="T82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
+        <v>305</v>
+      </c>
+      <c r="C83" t="s">
+        <v>306</v>
+      </c>
+      <c r="S83">
+        <v>1</v>
+      </c>
+      <c r="T83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>307</v>
+      </c>
+      <c r="C84" t="s">
+        <v>308</v>
+      </c>
+      <c r="S84">
+        <v>1</v>
+      </c>
+      <c r="T84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>309</v>
+      </c>
+      <c r="C85" t="s">
+        <v>310</v>
+      </c>
+      <c r="S85">
+        <v>1</v>
+      </c>
+      <c r="T85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>311</v>
+      </c>
+      <c r="C86" t="s">
+        <v>312</v>
+      </c>
+      <c r="S86">
+        <v>1</v>
+      </c>
+      <c r="T86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>313</v>
+      </c>
+      <c r="C87" t="s">
+        <v>314</v>
+      </c>
+      <c r="S87">
+        <v>1</v>
+      </c>
+      <c r="T87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>88</v>
+      </c>
+      <c r="B88" t="s">
+        <v>315</v>
+      </c>
+      <c r="C88" t="s">
+        <v>316</v>
+      </c>
+      <c r="S88">
+        <v>1</v>
+      </c>
+      <c r="T88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
+        <v>317</v>
+      </c>
+      <c r="C89" t="s">
+        <v>318</v>
+      </c>
+      <c r="S89">
+        <v>1</v>
+      </c>
+      <c r="T89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
+        <v>319</v>
+      </c>
+      <c r="C90" t="s">
+        <v>320</v>
+      </c>
+      <c r="S90">
+        <v>1</v>
+      </c>
+      <c r="T90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>91</v>
+      </c>
+      <c r="B91" t="s">
+        <v>322</v>
+      </c>
+      <c r="C91" t="s">
+        <v>321</v>
+      </c>
+      <c r="S91">
+        <v>1</v>
+      </c>
+      <c r="T91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>92</v>
+      </c>
+      <c r="B92" t="s">
+        <v>323</v>
+      </c>
+      <c r="C92" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add match protocol download
</commit_message>
<xml_diff>
--- a/database/_legacy-data/clubs.xlsx
+++ b/database/_legacy-data/clubs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20685" yWindow="0" windowWidth="3360" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21825" yWindow="0" windowWidth="3360" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mannschaft" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1665" uniqueCount="366">
   <si>
     <t>Dritte III</t>
   </si>
@@ -1966,10 +1966,10 @@
   <dimension ref="A1:V105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q60" sqref="Q60"/>
+      <selection pane="bottomRight" activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2125,11 +2125,11 @@
       </c>
       <c r="U2" s="2">
         <f ca="1">NOW()</f>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V2" s="2">
         <f ca="1">NOW()</f>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -2195,11 +2195,11 @@
       </c>
       <c r="U3" s="2">
         <f t="shared" ref="U3:V66" ca="1" si="0">NOW()</f>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -2265,11 +2265,11 @@
       </c>
       <c r="U4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -2335,11 +2335,11 @@
       </c>
       <c r="U5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -2405,11 +2405,11 @@
       </c>
       <c r="U6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -2475,11 +2475,11 @@
       </c>
       <c r="U7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -2545,11 +2545,11 @@
       </c>
       <c r="U8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -2615,11 +2615,11 @@
       </c>
       <c r="U9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -2685,11 +2685,11 @@
       </c>
       <c r="U10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -2755,11 +2755,11 @@
       </c>
       <c r="U11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -2825,11 +2825,11 @@
       </c>
       <c r="U12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -2895,11 +2895,11 @@
       </c>
       <c r="U13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -2965,11 +2965,11 @@
       </c>
       <c r="U14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -3035,11 +3035,11 @@
       </c>
       <c r="U15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -3105,11 +3105,11 @@
       </c>
       <c r="U16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -3175,11 +3175,11 @@
       </c>
       <c r="U17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -3245,11 +3245,11 @@
       </c>
       <c r="U18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
@@ -3315,11 +3315,11 @@
       </c>
       <c r="U19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -3385,11 +3385,11 @@
       </c>
       <c r="U20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -3455,11 +3455,11 @@
       </c>
       <c r="U21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
@@ -3525,11 +3525,11 @@
       </c>
       <c r="U22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
@@ -3595,11 +3595,11 @@
       </c>
       <c r="U23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -3665,11 +3665,11 @@
       </c>
       <c r="U24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -3735,11 +3735,11 @@
       </c>
       <c r="U25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -3805,11 +3805,11 @@
       </c>
       <c r="U26" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V26" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
@@ -3875,11 +3875,11 @@
       </c>
       <c r="U27" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V27" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
@@ -3945,11 +3945,11 @@
       </c>
       <c r="U28" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V28" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
@@ -4015,11 +4015,11 @@
       </c>
       <c r="U29" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V29" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
@@ -4085,11 +4085,11 @@
       </c>
       <c r="U30" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V30" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
@@ -4155,11 +4155,11 @@
       </c>
       <c r="U31" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V31" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
@@ -4225,11 +4225,11 @@
       </c>
       <c r="U32" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V32" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
@@ -4295,11 +4295,11 @@
       </c>
       <c r="U33" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V33" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
@@ -4365,11 +4365,11 @@
       </c>
       <c r="U34" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V34" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
@@ -4435,11 +4435,11 @@
       </c>
       <c r="U35" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V35" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
@@ -4505,11 +4505,11 @@
       </c>
       <c r="U36" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V36" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
@@ -4575,11 +4575,11 @@
       </c>
       <c r="U37" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V37" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
@@ -4645,11 +4645,11 @@
       </c>
       <c r="U38" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V38" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
@@ -4715,11 +4715,11 @@
       </c>
       <c r="U39" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V39" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
@@ -4785,11 +4785,11 @@
       </c>
       <c r="U40" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V40" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
@@ -4855,11 +4855,11 @@
       </c>
       <c r="U41" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V41" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
@@ -4925,11 +4925,11 @@
       </c>
       <c r="U42" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V42" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
@@ -4995,11 +4995,11 @@
       </c>
       <c r="U43" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V43" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
@@ -5065,11 +5065,11 @@
       </c>
       <c r="U44" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V44" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
@@ -5135,11 +5135,11 @@
       </c>
       <c r="U45" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V45" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
@@ -5205,11 +5205,11 @@
       </c>
       <c r="U46" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V46" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
@@ -5275,11 +5275,11 @@
       </c>
       <c r="U47" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V47" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
@@ -5345,11 +5345,11 @@
       </c>
       <c r="U48" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V48" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
@@ -5415,11 +5415,11 @@
       </c>
       <c r="U49" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V49" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
@@ -5485,11 +5485,11 @@
       </c>
       <c r="U50" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V50" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
@@ -5555,11 +5555,11 @@
       </c>
       <c r="U51" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V51" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
@@ -5625,11 +5625,11 @@
       </c>
       <c r="U52" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V52" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
@@ -5695,11 +5695,11 @@
       </c>
       <c r="U53" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V53" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
@@ -5765,11 +5765,11 @@
       </c>
       <c r="U54" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V54" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
@@ -5835,11 +5835,11 @@
       </c>
       <c r="U55" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V55" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
@@ -5905,11 +5905,11 @@
       </c>
       <c r="U56" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V56" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
@@ -5975,11 +5975,11 @@
       </c>
       <c r="U57" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V57" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
@@ -6045,11 +6045,11 @@
       </c>
       <c r="U58" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V58" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
@@ -6115,11 +6115,11 @@
       </c>
       <c r="U59" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V59" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
@@ -6185,11 +6185,11 @@
       </c>
       <c r="U60" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V60" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
@@ -6255,11 +6255,11 @@
       </c>
       <c r="U61" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V61" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
@@ -6325,11 +6325,11 @@
       </c>
       <c r="U62" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V62" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
@@ -6395,11 +6395,11 @@
       </c>
       <c r="U63" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V63" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
@@ -6465,11 +6465,11 @@
       </c>
       <c r="U64" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V64" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.25">
@@ -6535,11 +6535,11 @@
       </c>
       <c r="U65" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V65" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
@@ -6605,11 +6605,11 @@
       </c>
       <c r="U66" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V66" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.25">
@@ -6675,11 +6675,11 @@
       </c>
       <c r="U67" s="2">
         <f t="shared" ref="U67:V105" ca="1" si="1">NOW()</f>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V67" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.25">
@@ -6745,11 +6745,11 @@
       </c>
       <c r="U68" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V68" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.25">
@@ -6777,8 +6777,8 @@
       <c r="H69" s="1">
         <v>42370</v>
       </c>
-      <c r="I69" s="1" t="s">
-        <v>350</v>
+      <c r="I69" s="1">
+        <v>43100</v>
       </c>
       <c r="J69" t="s">
         <v>350</v>
@@ -6815,11 +6815,11 @@
       </c>
       <c r="U69" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V69" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
@@ -6885,11 +6885,11 @@
       </c>
       <c r="U70" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V70" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
@@ -6955,11 +6955,11 @@
       </c>
       <c r="U71" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V71" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.25">
@@ -7025,11 +7025,11 @@
       </c>
       <c r="U72" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V72" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
@@ -7095,11 +7095,11 @@
       </c>
       <c r="U73" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V73" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
@@ -7165,11 +7165,11 @@
       </c>
       <c r="U74" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V74" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.25">
@@ -7235,11 +7235,11 @@
       </c>
       <c r="U75" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V75" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
@@ -7305,11 +7305,11 @@
       </c>
       <c r="U76" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V76" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.25">
@@ -7375,11 +7375,11 @@
       </c>
       <c r="U77" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V77" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.25">
@@ -7445,11 +7445,11 @@
       </c>
       <c r="U78" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V78" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.25">
@@ -7515,11 +7515,11 @@
       </c>
       <c r="U79" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V79" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.25">
@@ -7585,11 +7585,11 @@
       </c>
       <c r="U80" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V80" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.25">
@@ -7655,11 +7655,11 @@
       </c>
       <c r="U81" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V81" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.25">
@@ -7725,11 +7725,11 @@
       </c>
       <c r="U82" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V82" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.25">
@@ -7795,11 +7795,11 @@
       </c>
       <c r="U83" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V83" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.25">
@@ -7865,11 +7865,11 @@
       </c>
       <c r="U84" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V84" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.25">
@@ -7935,11 +7935,11 @@
       </c>
       <c r="U85" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V85" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.25">
@@ -8005,11 +8005,11 @@
       </c>
       <c r="U86" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V86" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.25">
@@ -8075,11 +8075,11 @@
       </c>
       <c r="U87" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V87" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.25">
@@ -8145,11 +8145,11 @@
       </c>
       <c r="U88" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V88" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.25">
@@ -8215,11 +8215,11 @@
       </c>
       <c r="U89" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V89" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.25">
@@ -8285,11 +8285,11 @@
       </c>
       <c r="U90" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V90" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="91" spans="1:22" x14ac:dyDescent="0.25">
@@ -8355,11 +8355,11 @@
       </c>
       <c r="U91" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V91" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.25">
@@ -8425,11 +8425,11 @@
       </c>
       <c r="U92" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V92" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.25">
@@ -8495,11 +8495,11 @@
       </c>
       <c r="U93" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V93" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="94" spans="1:22" x14ac:dyDescent="0.25">
@@ -8565,11 +8565,11 @@
       </c>
       <c r="U94" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V94" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="95" spans="1:22" x14ac:dyDescent="0.25">
@@ -8635,11 +8635,11 @@
       </c>
       <c r="U95" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V95" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="96" spans="1:22" x14ac:dyDescent="0.25">
@@ -8705,11 +8705,11 @@
       </c>
       <c r="U96" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V96" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="97" spans="1:22" x14ac:dyDescent="0.25">
@@ -8775,11 +8775,11 @@
       </c>
       <c r="U97" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V97" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="98" spans="1:22" x14ac:dyDescent="0.25">
@@ -8845,11 +8845,11 @@
       </c>
       <c r="U98" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V98" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="99" spans="1:22" x14ac:dyDescent="0.25">
@@ -8915,11 +8915,11 @@
       </c>
       <c r="U99" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V99" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="100" spans="1:22" x14ac:dyDescent="0.25">
@@ -8985,11 +8985,11 @@
       </c>
       <c r="U100" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V100" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="101" spans="1:22" x14ac:dyDescent="0.25">
@@ -9055,11 +9055,11 @@
       </c>
       <c r="U101" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V101" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="102" spans="1:22" x14ac:dyDescent="0.25">
@@ -9125,11 +9125,11 @@
       </c>
       <c r="U102" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V102" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="103" spans="1:22" x14ac:dyDescent="0.25">
@@ -9195,11 +9195,11 @@
       </c>
       <c r="U103" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V103" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="104" spans="1:22" x14ac:dyDescent="0.25">
@@ -9265,11 +9265,11 @@
       </c>
       <c r="U104" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V104" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
     <row r="105" spans="1:22" x14ac:dyDescent="0.25">
@@ -9335,11 +9335,11 @@
       </c>
       <c r="U105" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
       <c r="V105" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>43129.685524768516</v>
+        <v>43130.902735648146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>